<commit_message>
Verification upload - kartik1
</commit_message>
<xml_diff>
--- a/kartik1.xlsx
+++ b/kartik1.xlsx
@@ -5,22 +5,98 @@
   <x:bookViews>
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
-  <x:sheets/>
+  <x:sheets>
+    <x:sheet name="SheetMap" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Login Page" sheetId="3" r:id="rId3"/>
+    <x:sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <x:sheet name="Lookup" sheetId="5" r:id="rId5"/>
+  </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <x:si>
+    <x:t>Login Page</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SheetMap</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TestsuiteName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ObjectName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Url</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UserId</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Password</x:t>
+  </x:si>
+  <x:si>
+    <x:t>new</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Case - Search</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Iteration Value</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Field Names</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Search By</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Person</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Account</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lookup Sheet</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TestSuiteName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Object</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ParentField</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Iteration</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ExcelSheet</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SheetName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sheet1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lookup</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="1">
+  <x:numFmts count="2">
     <x:numFmt numFmtId="0" formatCode=""/>
+    <x:numFmt numFmtId="1" formatCode="@"/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="8">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -28,13 +104,74 @@
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF0000FF"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:u val="single"/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF0000FF"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF008000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF0000FF"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:u val="single"/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF0000FF"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFFF00"/>
+        <x:bgColor rgb="FFFFFF00"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -56,13 +193,76 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="1" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -71,6 +271,17 @@
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
 </x:styleSheet>
+</file>
+
+<file path=xl/tables/table.xml><?xml version="1.0" encoding="utf-8"?>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
+  <x:autoFilter ref="A1:B4"/>
+  <x:tableColumns count="2">
+    <x:tableColumn id="1" name="ExcelSheet"/>
+    <x:tableColumn id="2" name="SheetName"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,4 +565,263 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B4"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="12.700625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.410625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2">
+      <x:c r="A2" s="9" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="9" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="9" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="A2" location="'Login Page'!A1" tooltip="Go to Login Page" display="Login Page"/>
+    <x:hyperlink ref="A3" location="'Sheet1'!A1" tooltip="Go to Sheet1" display="Sheet1"/>
+    <x:hyperlink ref="A4" location="'Lookup'!A1" tooltip="Go to Lookup" display="Lookup"/>
+  </x:hyperlinks>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="1">
+    <x:tablePart r:id="rId8"/>
+  </x:tableParts>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F3"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s"/>
+      <x:c r="C1" s="2" t="s"/>
+      <x:c r="D1" s="2" t="s"/>
+      <x:c r="E1" s="2" t="s"/>
+      <x:c r="F1" s="3" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="4" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C2" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D2" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E2" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s"/>
+      <x:c r="D3" s="2" t="s"/>
+      <x:c r="E3" s="2" t="s"/>
+      <x:c r="F3" s="2" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="F1" location="'SheetMap'!A1" tooltip="Go to SheetMap" display="SheetMap"/>
+  </x:hyperlinks>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F4"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="3" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s"/>
+      <x:c r="C1" s="2" t="s"/>
+      <x:c r="D1" s="2" t="s"/>
+      <x:c r="E1" s="2" t="s"/>
+      <x:c r="F1" s="3" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C2" s="4" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s"/>
+      <x:c r="E2" s="2" t="s"/>
+      <x:c r="F2" s="2" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="5" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s"/>
+      <x:c r="C3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="2" t="s"/>
+      <x:c r="B4" s="6" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s"/>
+      <x:c r="D4" s="2" t="s"/>
+      <x:c r="E4" s="2" t="s"/>
+      <x:c r="F4" s="2" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="F1" location="'SheetMap'!A1" tooltip="Go to SheetMap" display="SheetMap"/>
+  </x:hyperlinks>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F2"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="7" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s"/>
+      <x:c r="C1" s="2" t="s"/>
+      <x:c r="D1" s="2" t="s"/>
+      <x:c r="E1" s="2" t="s"/>
+      <x:c r="F1" s="3" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="8" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B2" s="8" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C2" s="8" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D2" s="8" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E2" s="8" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="F1" location="'SheetMap'!A1" tooltip="Go to SheetMap" display="SheetMap"/>
+  </x:hyperlinks>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>